<commit_message>
données inventaire du mois de septembre modifié par infotech
</commit_message>
<xml_diff>
--- a/correspondances.xlsx
+++ b/correspondances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LP\Desktop\dashbord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47768874-6A93-44FF-8584-69DAD2FD84FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD56DD7C-0206-4D14-95B0-B6632CB1B6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9270" yWindow="1350" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="290">
   <si>
     <t>Catégorie</t>
   </si>
@@ -980,6 +980,24 @@
   </si>
   <si>
     <t>MOET CHANDON ROSE</t>
+  </si>
+  <si>
+    <t>DOM PERIGNON</t>
+  </si>
+  <si>
+    <t>HENNESSY 35CL</t>
+  </si>
+  <si>
+    <t>REMY MARTIN VSOP BTL</t>
+  </si>
+  <si>
+    <t>JET 27</t>
+  </si>
+  <si>
+    <t>JET 27 BTL</t>
+  </si>
+  <si>
+    <t>THE</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1124,6 +1142,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C302" sqref="C302"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="B313" sqref="B313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -4722,6 +4743,72 @@
         <v>281</v>
       </c>
     </row>
+    <row r="302" spans="1:3">
+      <c r="A302" t="s">
+        <v>3</v>
+      </c>
+      <c r="B302" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C302" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" t="s">
+        <v>3</v>
+      </c>
+      <c r="B303" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C303" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304" t="s">
+        <v>3</v>
+      </c>
+      <c r="B304" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C304" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305" t="s">
+        <v>3</v>
+      </c>
+      <c r="B305" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C305" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" t="s">
+        <v>3</v>
+      </c>
+      <c r="B306" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C306" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307" t="s">
+        <v>3</v>
+      </c>
+      <c r="B307" t="s">
+        <v>127</v>
+      </c>
+      <c r="C307" t="s">
+        <v>289</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C301" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>